<commit_message>
Tablas actualizadas 1-dic + probador de todas las cadenas
</commit_message>
<xml_diff>
--- a/Parseador de Tablas/ACCION-GOTO.xlsx
+++ b/Parseador de Tablas/ACCION-GOTO.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="157">
   <si>
     <t>A</t>
   </si>
@@ -310,6 +310,9 @@
     <t>r34</t>
   </si>
   <si>
+    <t>r17</t>
+  </si>
+  <si>
     <t>r21</t>
   </si>
   <si>
@@ -397,16 +400,16 @@
     <t>r14</t>
   </si>
   <si>
-    <t>r15</t>
+    <t>d98</t>
   </si>
   <si>
-    <t>r16</t>
-  </si>
-  <si>
-    <t>r17</t>
+    <t>d100</t>
   </si>
   <si>
     <t>d32</t>
+  </si>
+  <si>
+    <t>r18</t>
   </si>
   <si>
     <t>d77</t>
@@ -469,7 +472,16 @@
     <t>r28</t>
   </si>
   <si>
+    <t>d99</t>
+  </si>
+  <si>
+    <t>r15</t>
+  </si>
+  <si>
     <t>r13</t>
+  </si>
+  <si>
+    <t>r16</t>
   </si>
 </sst>
 </file>
@@ -510,7 +522,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -549,6 +561,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE5CD"/>
+        <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFE599"/>
         <bgColor rgb="FFFFE599"/>
       </patternFill>
@@ -560,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -606,13 +630,16 @@
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="7" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2843,7 +2870,7 @@
       <c r="BA27" s="6"/>
     </row>
     <row r="28">
-      <c r="A28" s="11">
+      <c r="A28" s="15">
         <v>25.0</v>
       </c>
       <c r="B28" s="2"/>
@@ -2902,7 +2929,7 @@
       <c r="BA28" s="6"/>
     </row>
     <row r="29">
-      <c r="A29" s="11">
+      <c r="A29" s="15">
         <v>26.0</v>
       </c>
       <c r="B29" s="2"/>
@@ -2971,7 +2998,7 @@
       <c r="BA29" s="6"/>
     </row>
     <row r="30">
-      <c r="A30" s="11">
+      <c r="A30" s="15">
         <v>27.0</v>
       </c>
       <c r="B30" s="2"/>
@@ -3040,7 +3067,7 @@
       <c r="BA30" s="6"/>
     </row>
     <row r="31">
-      <c r="A31" s="11">
+      <c r="A31" s="15">
         <v>28.0</v>
       </c>
       <c r="B31" s="2"/>
@@ -3109,7 +3136,7 @@
       <c r="BA31" s="6"/>
     </row>
     <row r="32">
-      <c r="A32" s="11">
+      <c r="A32" s="15">
         <v>29.0</v>
       </c>
       <c r="B32" s="2"/>
@@ -3178,7 +3205,7 @@
       <c r="BA32" s="6"/>
     </row>
     <row r="33">
-      <c r="A33" s="11">
+      <c r="A33" s="15">
         <v>30.0</v>
       </c>
       <c r="B33" s="2"/>
@@ -3245,133 +3272,151 @@
       <c r="BA33" s="6"/>
     </row>
     <row r="34">
-      <c r="A34" s="15">
+      <c r="A34" s="16">
         <v>31.0</v>
       </c>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="16" t="s">
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="2"/>
+      <c r="L34" s="2"/>
+      <c r="M34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="N34" s="6"/>
-      <c r="O34" s="16" t="s">
+      <c r="N34" s="2"/>
+      <c r="O34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
-      <c r="S34" s="6"/>
-      <c r="T34" s="6"/>
-      <c r="U34" s="16" t="s">
+      <c r="P34" s="2"/>
+      <c r="Q34" s="2"/>
+      <c r="R34" s="2"/>
+      <c r="S34" s="2"/>
+      <c r="T34" s="2"/>
+      <c r="U34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="V34" s="16" t="s">
+      <c r="V34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="W34" s="6"/>
-      <c r="X34" s="6"/>
-      <c r="Y34" s="6"/>
-      <c r="Z34" s="16" t="s">
+      <c r="W34" s="2"/>
+      <c r="X34" s="2"/>
+      <c r="Y34" s="2"/>
+      <c r="Z34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AA34" s="6"/>
-      <c r="AB34" s="6"/>
-      <c r="AC34" s="16" t="s">
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="12" t="s">
         <v>98</v>
       </c>
-      <c r="AD34" s="6"/>
-      <c r="AE34" s="6"/>
-      <c r="AF34" s="6"/>
-      <c r="AG34" s="6"/>
-      <c r="AH34" s="6"/>
-      <c r="AI34" s="6"/>
-      <c r="AJ34" s="6"/>
-      <c r="AK34" s="6"/>
-      <c r="AL34" s="6"/>
-      <c r="AM34" s="6"/>
-      <c r="AN34" s="6"/>
-      <c r="AO34" s="6"/>
-      <c r="AP34" s="6"/>
-      <c r="AQ34" s="6"/>
-      <c r="AR34" s="6"/>
-      <c r="AS34" s="6"/>
-      <c r="AT34" s="6"/>
-      <c r="AU34" s="6"/>
-      <c r="AV34" s="6"/>
-      <c r="AW34" s="6"/>
+      <c r="AD34" s="4"/>
+      <c r="AE34" s="4"/>
+      <c r="AF34" s="4"/>
+      <c r="AG34" s="4"/>
+      <c r="AH34" s="4"/>
+      <c r="AI34" s="4"/>
+      <c r="AJ34" s="4"/>
+      <c r="AK34" s="4"/>
+      <c r="AL34" s="4"/>
+      <c r="AM34" s="4"/>
+      <c r="AN34" s="4"/>
+      <c r="AO34" s="4"/>
+      <c r="AP34" s="4"/>
+      <c r="AQ34" s="4"/>
+      <c r="AR34" s="4"/>
+      <c r="AS34" s="4"/>
+      <c r="AT34" s="4"/>
+      <c r="AU34" s="4"/>
+      <c r="AV34" s="4"/>
+      <c r="AW34" s="4"/>
       <c r="AX34" s="6"/>
       <c r="AY34" s="6"/>
       <c r="AZ34" s="6"/>
       <c r="BA34" s="6"/>
     </row>
     <row r="35">
-      <c r="A35" s="16">
+      <c r="A35" s="17">
         <v>32.0</v>
       </c>
-      <c r="B35" s="17"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="16"/>
-      <c r="N35" s="17"/>
-      <c r="O35" s="16"/>
-      <c r="P35" s="17"/>
-      <c r="Q35" s="17"/>
-      <c r="R35" s="17"/>
-      <c r="S35" s="17"/>
-      <c r="T35" s="17"/>
-      <c r="U35" s="16"/>
-      <c r="V35" s="16"/>
-      <c r="W35" s="17"/>
-      <c r="X35" s="17"/>
-      <c r="Y35" s="17"/>
-      <c r="Z35" s="16"/>
-      <c r="AA35" s="17"/>
-      <c r="AB35" s="17"/>
-      <c r="AC35" s="16"/>
-      <c r="AD35" s="17"/>
-      <c r="AE35" s="17"/>
-      <c r="AF35" s="17"/>
-      <c r="AG35" s="17"/>
-      <c r="AH35" s="17"/>
-      <c r="AI35" s="17"/>
-      <c r="AJ35" s="17"/>
-      <c r="AK35" s="17"/>
-      <c r="AL35" s="17"/>
-      <c r="AM35" s="17"/>
-      <c r="AN35" s="17"/>
-      <c r="AO35" s="17"/>
-      <c r="AP35" s="17"/>
-      <c r="AQ35" s="17"/>
-      <c r="AR35" s="17"/>
-      <c r="AS35" s="17"/>
-      <c r="AT35" s="17"/>
-      <c r="AU35" s="17"/>
-      <c r="AV35" s="17"/>
-      <c r="AW35" s="17"/>
-      <c r="AX35" s="17"/>
-      <c r="AY35" s="17"/>
-      <c r="AZ35" s="17"/>
-      <c r="BA35" s="17"/>
+      <c r="B35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="C35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="L35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="M35" s="12"/>
+      <c r="N35" s="2"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="12"/>
+      <c r="V35" s="12"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
+      <c r="Y35" s="2"/>
+      <c r="Z35" s="12"/>
+      <c r="AA35" s="2"/>
+      <c r="AB35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AC35" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD35" s="4"/>
+      <c r="AE35" s="4"/>
+      <c r="AF35" s="4"/>
+      <c r="AG35" s="4"/>
+      <c r="AH35" s="4"/>
+      <c r="AI35" s="4"/>
+      <c r="AJ35" s="4"/>
+      <c r="AK35" s="4"/>
+      <c r="AL35" s="4"/>
+      <c r="AM35" s="4"/>
+      <c r="AN35" s="4"/>
+      <c r="AO35" s="4"/>
+      <c r="AP35" s="4"/>
+      <c r="AQ35" s="4"/>
+      <c r="AR35" s="4"/>
+      <c r="AS35" s="4"/>
+      <c r="AT35" s="4"/>
+      <c r="AU35" s="4"/>
+      <c r="AV35" s="4"/>
+      <c r="AW35" s="4"/>
+      <c r="AX35" s="18"/>
+      <c r="AY35" s="18"/>
+      <c r="AZ35" s="18"/>
+      <c r="BA35" s="18"/>
     </row>
     <row r="36">
-      <c r="A36" s="11">
+      <c r="A36" s="15">
         <v>33.0</v>
       </c>
       <c r="B36" s="2"/>
@@ -3448,7 +3493,7 @@
       <c r="BA36" s="6"/>
     </row>
     <row r="37">
-      <c r="A37" s="11">
+      <c r="A37" s="15">
         <v>34.0</v>
       </c>
       <c r="B37" s="2"/>
@@ -3463,7 +3508,7 @@
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
       <c r="M37" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="N37" s="2"/>
       <c r="O37" s="12" t="s">
@@ -3475,21 +3520,21 @@
       <c r="S37" s="2"/>
       <c r="T37" s="2"/>
       <c r="U37" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="V37" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="W37" s="2"/>
       <c r="X37" s="2"/>
       <c r="Y37" s="2"/>
       <c r="Z37" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AA37" s="2"/>
       <c r="AB37" s="2"/>
       <c r="AC37" s="12" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="AD37" s="4"/>
       <c r="AE37" s="4"/>
@@ -3517,7 +3562,7 @@
       <c r="BA37" s="6"/>
     </row>
     <row r="38">
-      <c r="A38" s="11">
+      <c r="A38" s="15">
         <v>35.0</v>
       </c>
       <c r="B38" s="2"/>
@@ -3532,7 +3577,7 @@
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
       <c r="M38" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="N38" s="2"/>
       <c r="O38" s="12" t="s">
@@ -3544,21 +3589,21 @@
       <c r="S38" s="2"/>
       <c r="T38" s="2"/>
       <c r="U38" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="V38" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="W38" s="2"/>
       <c r="X38" s="2"/>
       <c r="Y38" s="2"/>
       <c r="Z38" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AA38" s="2"/>
       <c r="AB38" s="2"/>
       <c r="AC38" s="12" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="AD38" s="4"/>
       <c r="AE38" s="4"/>
@@ -3586,7 +3631,7 @@
       <c r="BA38" s="6"/>
     </row>
     <row r="39">
-      <c r="A39" s="11">
+      <c r="A39" s="15">
         <v>36.0</v>
       </c>
       <c r="B39" s="2"/>
@@ -3657,7 +3702,7 @@
       <c r="BA39" s="6"/>
     </row>
     <row r="40">
-      <c r="A40" s="11">
+      <c r="A40" s="15">
         <v>37.0</v>
       </c>
       <c r="B40" s="2"/>
@@ -3672,11 +3717,11 @@
       <c r="K40" s="2"/>
       <c r="L40" s="2"/>
       <c r="M40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
@@ -3684,21 +3729,21 @@
       <c r="S40" s="2"/>
       <c r="T40" s="2"/>
       <c r="U40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="V40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="W40" s="2"/>
       <c r="X40" s="2"/>
       <c r="Y40" s="2"/>
       <c r="Z40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AA40" s="2"/>
       <c r="AB40" s="2"/>
       <c r="AC40" s="12" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="AD40" s="4"/>
       <c r="AE40" s="4"/>
@@ -3726,7 +3771,7 @@
       <c r="BA40" s="6"/>
     </row>
     <row r="41">
-      <c r="A41" s="11">
+      <c r="A41" s="15">
         <v>38.0</v>
       </c>
       <c r="B41" s="2"/>
@@ -3811,7 +3856,7 @@
       <c r="BA41" s="6"/>
     </row>
     <row r="42">
-      <c r="A42" s="11">
+      <c r="A42" s="15">
         <v>39.0</v>
       </c>
       <c r="B42" s="2"/>
@@ -3834,14 +3879,14 @@
       <c r="S42" s="2"/>
       <c r="T42" s="2"/>
       <c r="U42" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="V42" s="2"/>
       <c r="W42" s="2"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="2"/>
       <c r="Z42" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AA42" s="2"/>
       <c r="AB42" s="2"/>
@@ -3874,7 +3919,7 @@
       <c r="BA42" s="6"/>
     </row>
     <row r="43">
-      <c r="A43" s="11">
+      <c r="A43" s="15">
         <v>40.0</v>
       </c>
       <c r="B43" s="2"/>
@@ -3902,7 +3947,7 @@
       <c r="X43" s="2"/>
       <c r="Y43" s="2"/>
       <c r="Z43" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="AA43" s="2"/>
       <c r="AB43" s="2"/>
@@ -3933,7 +3978,7 @@
       <c r="BA43" s="6"/>
     </row>
     <row r="44">
-      <c r="A44" s="11">
+      <c r="A44" s="15">
         <v>41.0</v>
       </c>
       <c r="B44" s="2"/>
@@ -3961,7 +4006,7 @@
       <c r="X44" s="2"/>
       <c r="Y44" s="2"/>
       <c r="Z44" s="12" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="AA44" s="2"/>
       <c r="AB44" s="2"/>
@@ -3992,7 +4037,7 @@
       <c r="BA44" s="6"/>
     </row>
     <row r="45">
-      <c r="A45" s="11">
+      <c r="A45" s="15">
         <v>42.0</v>
       </c>
       <c r="B45" s="2"/>
@@ -4007,11 +4052,11 @@
       <c r="K45" s="2"/>
       <c r="L45" s="2"/>
       <c r="M45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
@@ -4019,21 +4064,21 @@
       <c r="S45" s="2"/>
       <c r="T45" s="2"/>
       <c r="U45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="V45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="W45" s="2"/>
       <c r="X45" s="2"/>
       <c r="Y45" s="2"/>
       <c r="Z45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AA45" s="2"/>
       <c r="AB45" s="2"/>
       <c r="AC45" s="12" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="AD45" s="4"/>
       <c r="AE45" s="4"/>
@@ -4061,7 +4106,7 @@
       <c r="BA45" s="6"/>
     </row>
     <row r="46">
-      <c r="A46" s="11">
+      <c r="A46" s="15">
         <v>43.0</v>
       </c>
       <c r="B46" s="2"/>
@@ -4084,14 +4129,14 @@
       <c r="S46" s="2"/>
       <c r="T46" s="2"/>
       <c r="U46" s="12" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="V46" s="2"/>
       <c r="W46" s="2"/>
       <c r="X46" s="2"/>
       <c r="Y46" s="2"/>
       <c r="Z46" s="12" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="AA46" s="2"/>
       <c r="AB46" s="2"/>
@@ -4124,7 +4169,7 @@
       <c r="BA46" s="6"/>
     </row>
     <row r="47">
-      <c r="A47" s="11">
+      <c r="A47" s="15">
         <v>44.0</v>
       </c>
       <c r="B47" s="2"/>
@@ -4152,7 +4197,7 @@
       <c r="X47" s="2"/>
       <c r="Y47" s="2"/>
       <c r="Z47" s="12" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="AA47" s="2"/>
       <c r="AB47" s="2"/>
@@ -4183,7 +4228,7 @@
       <c r="BA47" s="6"/>
     </row>
     <row r="48">
-      <c r="A48" s="11">
+      <c r="A48" s="15">
         <v>45.0</v>
       </c>
       <c r="B48" s="2"/>
@@ -4266,7 +4311,7 @@
       <c r="BA48" s="6"/>
     </row>
     <row r="49">
-      <c r="A49" s="11">
+      <c r="A49" s="15">
         <v>46.0</v>
       </c>
       <c r="B49" s="2"/>
@@ -4277,7 +4322,7 @@
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="12" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="J49" s="2"/>
       <c r="K49" s="2"/>
@@ -4325,7 +4370,7 @@
       <c r="BA49" s="6"/>
     </row>
     <row r="50">
-      <c r="A50" s="11">
+      <c r="A50" s="15">
         <v>47.0</v>
       </c>
       <c r="B50" s="2"/>
@@ -4349,7 +4394,7 @@
       <c r="T50" s="2"/>
       <c r="U50" s="2"/>
       <c r="V50" s="12" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="W50" s="2"/>
       <c r="X50" s="2"/>
@@ -4384,33 +4429,33 @@
       <c r="BA50" s="6"/>
     </row>
     <row r="51">
-      <c r="A51" s="11">
+      <c r="A51" s="15">
         <v>48.0</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="J51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="L51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="M51" s="2"/>
       <c r="N51" s="2"/>
@@ -4428,10 +4473,10 @@
       <c r="Z51" s="2"/>
       <c r="AA51" s="2"/>
       <c r="AB51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AC51" s="12" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AD51" s="4"/>
       <c r="AE51" s="4"/>
@@ -4459,7 +4504,7 @@
       <c r="BA51" s="6"/>
     </row>
     <row r="52">
-      <c r="A52" s="11">
+      <c r="A52" s="15">
         <v>49.0</v>
       </c>
       <c r="B52" s="2"/>
@@ -4470,7 +4515,7 @@
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J52" s="2"/>
       <c r="K52" s="2"/>
@@ -4488,13 +4533,13 @@
       <c r="W52" s="2"/>
       <c r="X52" s="2"/>
       <c r="Y52" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="2"/>
       <c r="AB52" s="2"/>
       <c r="AC52" s="12" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="AD52" s="4"/>
       <c r="AE52" s="4"/>
@@ -4522,7 +4567,7 @@
       <c r="BA52" s="6"/>
     </row>
     <row r="53">
-      <c r="A53" s="11">
+      <c r="A53" s="15">
         <v>50.0</v>
       </c>
       <c r="B53" s="12"/>
@@ -4533,7 +4578,7 @@
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="12" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
@@ -4551,13 +4596,13 @@
       <c r="W53" s="12"/>
       <c r="X53" s="12"/>
       <c r="Y53" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z53" s="12"/>
       <c r="AA53" s="12"/>
       <c r="AB53" s="12"/>
       <c r="AC53" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AD53" s="4"/>
       <c r="AE53" s="4"/>
@@ -4585,7 +4630,7 @@
       <c r="BA53" s="6"/>
     </row>
     <row r="54">
-      <c r="A54" s="11">
+      <c r="A54" s="15">
         <v>51.0</v>
       </c>
       <c r="B54" s="2"/>
@@ -4596,7 +4641,7 @@
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="J54" s="2"/>
       <c r="K54" s="2"/>
@@ -4614,13 +4659,13 @@
       <c r="W54" s="2"/>
       <c r="X54" s="2"/>
       <c r="Y54" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="2"/>
       <c r="AB54" s="2"/>
       <c r="AC54" s="12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="AD54" s="4"/>
       <c r="AE54" s="4"/>
@@ -4648,7 +4693,7 @@
       <c r="BA54" s="6"/>
     </row>
     <row r="55">
-      <c r="A55" s="11">
+      <c r="A55" s="15">
         <v>52.0</v>
       </c>
       <c r="B55" s="2"/>
@@ -4659,7 +4704,7 @@
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="12" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="J55" s="2"/>
       <c r="K55" s="2"/>
@@ -4707,14 +4752,14 @@
       <c r="BA55" s="6"/>
     </row>
     <row r="56">
-      <c r="A56" s="11">
+      <c r="A56" s="15">
         <v>53.0</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="12" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -4733,7 +4778,7 @@
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
       <c r="V56" s="12" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="W56" s="2"/>
       <c r="X56" s="2"/>
@@ -4770,7 +4815,7 @@
       <c r="BA56" s="6"/>
     </row>
     <row r="57">
-      <c r="A57" s="11">
+      <c r="A57" s="15">
         <v>54.0</v>
       </c>
       <c r="B57" s="2"/>
@@ -4853,7 +4898,7 @@
       <c r="BA57" s="6"/>
     </row>
     <row r="58">
-      <c r="A58" s="11">
+      <c r="A58" s="15">
         <v>55.0</v>
       </c>
       <c r="B58" s="2"/>
@@ -4877,7 +4922,7 @@
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
       <c r="V58" s="12" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="W58" s="2"/>
       <c r="X58" s="2"/>
@@ -4912,7 +4957,7 @@
       <c r="BA58" s="6"/>
     </row>
     <row r="59">
-      <c r="A59" s="11">
+      <c r="A59" s="15">
         <v>56.0</v>
       </c>
       <c r="B59" s="2"/>
@@ -4936,7 +4981,7 @@
       <c r="T59" s="2"/>
       <c r="U59" s="2"/>
       <c r="V59" s="12" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="W59" s="2"/>
       <c r="X59" s="2"/>
@@ -4971,7 +5016,7 @@
       <c r="BA59" s="6"/>
     </row>
     <row r="60">
-      <c r="A60" s="11">
+      <c r="A60" s="15">
         <v>57.0</v>
       </c>
       <c r="B60" s="2"/>
@@ -5054,7 +5099,7 @@
       <c r="BA60" s="6"/>
     </row>
     <row r="61">
-      <c r="A61" s="11">
+      <c r="A61" s="15">
         <v>58.0</v>
       </c>
       <c r="B61" s="2"/>
@@ -5078,7 +5123,7 @@
       <c r="T61" s="2"/>
       <c r="U61" s="2"/>
       <c r="V61" s="12" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="W61" s="2"/>
       <c r="X61" s="2"/>
@@ -5113,7 +5158,7 @@
       <c r="BA61" s="6"/>
     </row>
     <row r="62">
-      <c r="A62" s="11">
+      <c r="A62" s="15">
         <v>59.0</v>
       </c>
       <c r="B62" s="2"/>
@@ -5174,7 +5219,7 @@
       <c r="BA62" s="6"/>
     </row>
     <row r="63">
-      <c r="A63" s="11">
+      <c r="A63" s="15">
         <v>60.0</v>
       </c>
       <c r="B63" s="2"/>
@@ -5202,7 +5247,7 @@
       <c r="X63" s="2"/>
       <c r="Y63" s="2"/>
       <c r="Z63" s="12" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="AA63" s="2"/>
       <c r="AB63" s="2"/>
@@ -5233,7 +5278,7 @@
       <c r="BA63" s="6"/>
     </row>
     <row r="64">
-      <c r="A64" s="11">
+      <c r="A64" s="15">
         <v>61.0</v>
       </c>
       <c r="B64" s="2"/>
@@ -5258,7 +5303,7 @@
       <c r="U64" s="2"/>
       <c r="V64" s="2"/>
       <c r="W64" s="12" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="X64" s="2"/>
       <c r="Y64" s="2"/>
@@ -5292,7 +5337,7 @@
       <c r="BA64" s="6"/>
     </row>
     <row r="65">
-      <c r="A65" s="11">
+      <c r="A65" s="15">
         <v>62.0</v>
       </c>
       <c r="B65" s="2"/>
@@ -5320,7 +5365,7 @@
       <c r="V65" s="2"/>
       <c r="W65" s="2"/>
       <c r="X65" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y65" s="2"/>
       <c r="Z65" s="2"/>
@@ -5357,7 +5402,7 @@
       <c r="BA65" s="6"/>
     </row>
     <row r="66">
-      <c r="A66" s="11">
+      <c r="A66" s="15">
         <v>63.0</v>
       </c>
       <c r="B66" s="2"/>
@@ -5383,7 +5428,7 @@
       <c r="V66" s="2"/>
       <c r="W66" s="2"/>
       <c r="X66" s="12" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="Y66" s="2"/>
       <c r="Z66" s="2"/>
@@ -5416,33 +5461,33 @@
       <c r="BA66" s="6"/>
     </row>
     <row r="67">
-      <c r="A67" s="11">
+      <c r="A67" s="15">
         <v>64.0</v>
       </c>
       <c r="B67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="J67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="K67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="L67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="M67" s="2"/>
       <c r="N67" s="2"/>
@@ -5460,10 +5505,10 @@
       <c r="Z67" s="2"/>
       <c r="AA67" s="2"/>
       <c r="AB67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AC67" s="12" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="AD67" s="4"/>
       <c r="AE67" s="4"/>
@@ -5491,7 +5536,7 @@
       <c r="BA67" s="6"/>
     </row>
     <row r="68">
-      <c r="A68" s="11">
+      <c r="A68" s="15">
         <v>65.0</v>
       </c>
       <c r="B68" s="2"/>
@@ -5517,7 +5562,7 @@
       <c r="V68" s="2"/>
       <c r="W68" s="2"/>
       <c r="X68" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y68" s="2"/>
       <c r="Z68" s="2"/>
@@ -5554,7 +5599,7 @@
       <c r="BA68" s="6"/>
     </row>
     <row r="69">
-      <c r="A69" s="11">
+      <c r="A69" s="15">
         <v>66.0</v>
       </c>
       <c r="B69" s="2"/>
@@ -5637,7 +5682,7 @@
       <c r="BA69" s="6"/>
     </row>
     <row r="70">
-      <c r="A70" s="11">
+      <c r="A70" s="15">
         <v>67.0</v>
       </c>
       <c r="B70" s="2"/>
@@ -5722,7 +5767,7 @@
       <c r="BA70" s="6"/>
     </row>
     <row r="71">
-      <c r="A71" s="11">
+      <c r="A71" s="15">
         <v>68.0</v>
       </c>
       <c r="B71" s="2"/>
@@ -5750,7 +5795,7 @@
       <c r="X71" s="2"/>
       <c r="Y71" s="2"/>
       <c r="Z71" s="12" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="AA71" s="2"/>
       <c r="AB71" s="2"/>
@@ -5781,7 +5826,7 @@
       <c r="BA71" s="6"/>
     </row>
     <row r="72">
-      <c r="A72" s="11">
+      <c r="A72" s="15">
         <v>69.0</v>
       </c>
       <c r="B72" s="2"/>
@@ -5805,7 +5850,7 @@
       <c r="T72" s="2"/>
       <c r="U72" s="2"/>
       <c r="V72" s="12" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="W72" s="2"/>
       <c r="X72" s="2"/>
@@ -5840,33 +5885,33 @@
       <c r="BA72" s="6"/>
     </row>
     <row r="73">
-      <c r="A73" s="11">
+      <c r="A73" s="15">
         <v>70.0</v>
       </c>
       <c r="B73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E73" s="2"/>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="J73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="K73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="L73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="M73" s="2"/>
       <c r="N73" s="2"/>
@@ -5884,10 +5929,10 @@
       <c r="Z73" s="2"/>
       <c r="AA73" s="2"/>
       <c r="AB73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AC73" s="12" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="AD73" s="4"/>
       <c r="AE73" s="4"/>
@@ -5915,34 +5960,20 @@
       <c r="BA73" s="6"/>
     </row>
     <row r="74">
-      <c r="A74" s="11">
+      <c r="A74" s="17">
         <v>71.0</v>
       </c>
-      <c r="B74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="C74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D74" s="12" t="s">
-        <v>128</v>
-      </c>
+      <c r="B74" s="12"/>
+      <c r="C74" s="12"/>
+      <c r="D74" s="12"/>
       <c r="E74" s="2"/>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
-      <c r="I74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="J74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="K74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="L74" s="12" t="s">
-        <v>128</v>
-      </c>
+      <c r="I74" s="12"/>
+      <c r="J74" s="12"/>
+      <c r="K74" s="12"/>
+      <c r="L74" s="12"/>
       <c r="M74" s="2"/>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -5952,18 +5983,16 @@
       <c r="S74" s="2"/>
       <c r="T74" s="2"/>
       <c r="U74" s="2"/>
-      <c r="V74" s="2"/>
+      <c r="V74" s="12" t="s">
+        <v>129</v>
+      </c>
       <c r="W74" s="2"/>
       <c r="X74" s="2"/>
       <c r="Y74" s="2"/>
       <c r="Z74" s="2"/>
       <c r="AA74" s="2"/>
-      <c r="AB74" s="12" t="s">
-        <v>128</v>
-      </c>
-      <c r="AC74" s="12" t="s">
-        <v>128</v>
-      </c>
+      <c r="AB74" s="12"/>
+      <c r="AC74" s="12"/>
       <c r="AD74" s="4"/>
       <c r="AE74" s="4"/>
       <c r="AF74" s="4"/>
@@ -5990,34 +6019,20 @@
       <c r="BA74" s="6"/>
     </row>
     <row r="75">
-      <c r="A75" s="11">
+      <c r="A75" s="17">
         <v>72.0</v>
       </c>
-      <c r="B75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="C75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="D75" s="12" t="s">
-        <v>129</v>
-      </c>
+      <c r="B75" s="12"/>
+      <c r="C75" s="12"/>
+      <c r="D75" s="12"/>
       <c r="E75" s="2"/>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
-      <c r="I75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="J75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="K75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="L75" s="12" t="s">
-        <v>129</v>
-      </c>
+      <c r="I75" s="12"/>
+      <c r="J75" s="12"/>
+      <c r="K75" s="12"/>
+      <c r="L75" s="12"/>
       <c r="M75" s="2"/>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -6027,18 +6042,16 @@
       <c r="S75" s="2"/>
       <c r="T75" s="2"/>
       <c r="U75" s="2"/>
-      <c r="V75" s="2"/>
+      <c r="V75" s="12" t="s">
+        <v>130</v>
+      </c>
       <c r="W75" s="2"/>
       <c r="X75" s="2"/>
       <c r="Y75" s="2"/>
       <c r="Z75" s="2"/>
       <c r="AA75" s="2"/>
-      <c r="AB75" s="12" t="s">
-        <v>129</v>
-      </c>
-      <c r="AC75" s="12" t="s">
-        <v>129</v>
-      </c>
+      <c r="AB75" s="12"/>
+      <c r="AC75" s="12"/>
       <c r="AD75" s="4"/>
       <c r="AE75" s="4"/>
       <c r="AF75" s="4"/>
@@ -6065,34 +6078,20 @@
       <c r="BA75" s="6"/>
     </row>
     <row r="76">
-      <c r="A76" s="11">
+      <c r="A76" s="17">
         <v>73.0</v>
       </c>
-      <c r="B76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="C76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="D76" s="12" t="s">
-        <v>130</v>
-      </c>
+      <c r="B76" s="12"/>
+      <c r="C76" s="12"/>
+      <c r="D76" s="12"/>
       <c r="E76" s="2"/>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
-      <c r="I76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="K76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="L76" s="12" t="s">
-        <v>130</v>
-      </c>
+      <c r="I76" s="12"/>
+      <c r="J76" s="12"/>
+      <c r="K76" s="12"/>
+      <c r="L76" s="12"/>
       <c r="M76" s="2"/>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -6110,12 +6109,8 @@
       <c r="Y76" s="2"/>
       <c r="Z76" s="2"/>
       <c r="AA76" s="2"/>
-      <c r="AB76" s="12" t="s">
-        <v>130</v>
-      </c>
-      <c r="AC76" s="12" t="s">
-        <v>130</v>
-      </c>
+      <c r="AB76" s="12"/>
+      <c r="AC76" s="12"/>
       <c r="AD76" s="4"/>
       <c r="AE76" s="4"/>
       <c r="AF76" s="4"/>
@@ -6142,7 +6137,7 @@
       <c r="BA76" s="6"/>
     </row>
     <row r="77">
-      <c r="A77" s="11">
+      <c r="A77" s="17">
         <v>74.0</v>
       </c>
       <c r="B77" s="2"/>
@@ -6166,7 +6161,7 @@
       <c r="T77" s="2"/>
       <c r="U77" s="2"/>
       <c r="V77" s="12" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="W77" s="2"/>
       <c r="X77" s="2"/>
@@ -6201,7 +6196,7 @@
       <c r="BA77" s="6"/>
     </row>
     <row r="78">
-      <c r="A78" s="11">
+      <c r="A78" s="15">
         <v>75.0</v>
       </c>
       <c r="B78" s="2"/>
@@ -6227,7 +6222,7 @@
       <c r="V78" s="2"/>
       <c r="W78" s="2"/>
       <c r="X78" s="12" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="Y78" s="2"/>
       <c r="Z78" s="2"/>
@@ -6264,7 +6259,7 @@
       <c r="BA78" s="6"/>
     </row>
     <row r="79">
-      <c r="A79" s="11">
+      <c r="A79" s="15">
         <v>76.0</v>
       </c>
       <c r="B79" s="2"/>
@@ -6290,7 +6285,7 @@
       <c r="V79" s="2"/>
       <c r="W79" s="2"/>
       <c r="X79" s="12" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="Y79" s="2"/>
       <c r="Z79" s="2"/>
@@ -6323,33 +6318,33 @@
       <c r="BA79" s="6"/>
     </row>
     <row r="80">
-      <c r="A80" s="11">
+      <c r="A80" s="15">
         <v>77.0</v>
       </c>
       <c r="B80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="D80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E80" s="2"/>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="J80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="K80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="L80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="M80" s="2"/>
       <c r="N80" s="2"/>
@@ -6367,10 +6362,10 @@
       <c r="Z80" s="2"/>
       <c r="AA80" s="2"/>
       <c r="AB80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AC80" s="12" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="AD80" s="4"/>
       <c r="AE80" s="4"/>
@@ -6398,7 +6393,7 @@
       <c r="BA80" s="6"/>
     </row>
     <row r="81">
-      <c r="A81" s="11">
+      <c r="A81" s="15">
         <v>78.0</v>
       </c>
       <c r="B81" s="2"/>
@@ -6424,7 +6419,7 @@
       <c r="V81" s="2"/>
       <c r="W81" s="2"/>
       <c r="X81" s="12" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="Y81" s="2"/>
       <c r="Z81" s="2"/>
@@ -6457,7 +6452,7 @@
       <c r="BA81" s="6"/>
     </row>
     <row r="82">
-      <c r="A82" s="11">
+      <c r="A82" s="15">
         <v>79.0</v>
       </c>
       <c r="B82" s="2"/>
@@ -6491,7 +6486,7 @@
       <c r="X82" s="2"/>
       <c r="Y82" s="2"/>
       <c r="Z82" s="12" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="AA82" s="2"/>
       <c r="AB82" s="2"/>
@@ -6526,7 +6521,7 @@
       <c r="BA82" s="6"/>
     </row>
     <row r="83">
-      <c r="A83" s="11">
+      <c r="A83" s="15">
         <v>80.0</v>
       </c>
       <c r="B83" s="2"/>
@@ -6561,7 +6556,7 @@
       <c r="Y83" s="2"/>
       <c r="Z83" s="2"/>
       <c r="AA83" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AB83" s="2"/>
       <c r="AC83" s="2"/>
@@ -6595,7 +6590,7 @@
       <c r="BA83" s="6"/>
     </row>
     <row r="84">
-      <c r="A84" s="11">
+      <c r="A84" s="15">
         <v>81.0</v>
       </c>
       <c r="B84" s="2"/>
@@ -6623,7 +6618,7 @@
       <c r="X84" s="2"/>
       <c r="Y84" s="2"/>
       <c r="Z84" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="AA84" s="2"/>
       <c r="AB84" s="2"/>
@@ -6654,7 +6649,7 @@
       <c r="BA84" s="6"/>
     </row>
     <row r="85">
-      <c r="A85" s="11">
+      <c r="A85" s="15">
         <v>82.0</v>
       </c>
       <c r="B85" s="2"/>
@@ -6679,7 +6674,7 @@
       <c r="U85" s="2"/>
       <c r="V85" s="2"/>
       <c r="W85" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="X85" s="2"/>
       <c r="Y85" s="2"/>
@@ -6713,7 +6708,7 @@
       <c r="BA85" s="6"/>
     </row>
     <row r="86">
-      <c r="A86" s="11">
+      <c r="A86" s="15">
         <v>83.0</v>
       </c>
       <c r="B86" s="2"/>
@@ -6724,7 +6719,7 @@
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="J86" s="2"/>
       <c r="K86" s="2"/>
@@ -6772,7 +6767,7 @@
       <c r="BA86" s="6"/>
     </row>
     <row r="87">
-      <c r="A87" s="11">
+      <c r="A87" s="15">
         <v>84.0</v>
       </c>
       <c r="B87" s="2"/>
@@ -6795,14 +6790,14 @@
       <c r="S87" s="2"/>
       <c r="T87" s="2"/>
       <c r="U87" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V87" s="2"/>
       <c r="W87" s="2"/>
       <c r="X87" s="2"/>
       <c r="Y87" s="2"/>
       <c r="Z87" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AA87" s="2"/>
       <c r="AB87" s="2"/>
@@ -6835,7 +6830,7 @@
       <c r="BA87" s="6"/>
     </row>
     <row r="88">
-      <c r="A88" s="11">
+      <c r="A88" s="15">
         <v>85.0</v>
       </c>
       <c r="B88" s="2"/>
@@ -6862,7 +6857,7 @@
       <c r="W88" s="2"/>
       <c r="X88" s="2"/>
       <c r="Y88" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="Z88" s="2"/>
       <c r="AA88" s="2"/>
@@ -6894,7 +6889,7 @@
       <c r="BA88" s="6"/>
     </row>
     <row r="89">
-      <c r="A89" s="11">
+      <c r="A89" s="15">
         <v>86.0</v>
       </c>
       <c r="B89" s="2"/>
@@ -6921,7 +6916,7 @@
       <c r="W89" s="2"/>
       <c r="X89" s="2"/>
       <c r="Y89" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Z89" s="2"/>
       <c r="AA89" s="2"/>
@@ -6953,7 +6948,7 @@
       <c r="BA89" s="6"/>
     </row>
     <row r="90">
-      <c r="A90" s="11">
+      <c r="A90" s="15">
         <v>87.0</v>
       </c>
       <c r="B90" s="2"/>
@@ -6980,7 +6975,7 @@
       <c r="W90" s="2"/>
       <c r="X90" s="2"/>
       <c r="Y90" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="Z90" s="2"/>
       <c r="AA90" s="2"/>
@@ -7012,7 +7007,7 @@
       <c r="BA90" s="6"/>
     </row>
     <row r="91">
-      <c r="A91" s="11">
+      <c r="A91" s="15">
         <v>88.0</v>
       </c>
       <c r="B91" s="2"/>
@@ -7040,7 +7035,7 @@
       <c r="X91" s="2"/>
       <c r="Y91" s="2"/>
       <c r="Z91" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="AA91" s="2"/>
       <c r="AB91" s="2"/>
@@ -7071,7 +7066,7 @@
       <c r="BA91" s="6"/>
     </row>
     <row r="92">
-      <c r="A92" s="11">
+      <c r="A92" s="15">
         <v>89.0</v>
       </c>
       <c r="B92" s="2"/>
@@ -7136,7 +7131,7 @@
       <c r="BA92" s="6"/>
     </row>
     <row r="93">
-      <c r="A93" s="11">
+      <c r="A93" s="15">
         <v>90.0</v>
       </c>
       <c r="B93" s="2"/>
@@ -7147,7 +7142,7 @@
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="J93" s="2"/>
       <c r="K93" s="2"/>
@@ -7195,7 +7190,7 @@
       <c r="BA93" s="6"/>
     </row>
     <row r="94">
-      <c r="A94" s="11">
+      <c r="A94" s="15">
         <v>91.0</v>
       </c>
       <c r="B94" s="2"/>
@@ -7218,14 +7213,14 @@
       <c r="S94" s="2"/>
       <c r="T94" s="2"/>
       <c r="U94" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="V94" s="2"/>
       <c r="W94" s="2"/>
       <c r="X94" s="2"/>
       <c r="Y94" s="2"/>
       <c r="Z94" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="AA94" s="2"/>
       <c r="AB94" s="2"/>
@@ -7258,7 +7253,7 @@
       <c r="BA94" s="6"/>
     </row>
     <row r="95">
-      <c r="A95" s="11">
+      <c r="A95" s="15">
         <v>92.0</v>
       </c>
       <c r="B95" s="2"/>
@@ -7286,7 +7281,7 @@
       <c r="X95" s="2"/>
       <c r="Y95" s="2"/>
       <c r="Z95" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="AA95" s="2"/>
       <c r="AB95" s="2"/>
@@ -7317,7 +7312,7 @@
       <c r="BA95" s="6"/>
     </row>
     <row r="96">
-      <c r="A96" s="11">
+      <c r="A96" s="15">
         <v>93.0</v>
       </c>
       <c r="B96" s="12"/>
@@ -7348,7 +7343,7 @@
       <c r="AA96" s="2"/>
       <c r="AB96" s="2"/>
       <c r="AC96" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="AD96" s="4"/>
       <c r="AE96" s="4"/>
@@ -7376,33 +7371,33 @@
       <c r="BA96" s="6"/>
     </row>
     <row r="97">
-      <c r="A97" s="11">
+      <c r="A97" s="15">
         <v>94.0</v>
       </c>
       <c r="B97" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C97" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D97" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E97" s="2"/>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="J97" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="K97" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="L97" s="14" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="M97" s="2"/>
       <c r="N97" s="2"/>
@@ -7420,10 +7415,10 @@
       <c r="Z97" s="2"/>
       <c r="AA97" s="2"/>
       <c r="AB97" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AC97" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AD97" s="4"/>
       <c r="AE97" s="4"/>
@@ -7451,7 +7446,7 @@
       <c r="BA97" s="6"/>
     </row>
     <row r="98">
-      <c r="A98" s="11">
+      <c r="A98" s="15">
         <v>95.0</v>
       </c>
       <c r="B98" s="2"/>
@@ -7479,7 +7474,7 @@
       <c r="X98" s="2"/>
       <c r="Y98" s="2"/>
       <c r="Z98" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AA98" s="2"/>
       <c r="AB98" s="2"/>
@@ -7510,7 +7505,7 @@
       <c r="BA98" s="6"/>
     </row>
     <row r="99">
-      <c r="A99" s="11">
+      <c r="A99" s="15">
         <v>96.0</v>
       </c>
       <c r="B99" s="2"/>
@@ -7525,11 +7520,11 @@
       <c r="K99" s="2"/>
       <c r="L99" s="2"/>
       <c r="M99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="N99" s="2"/>
       <c r="O99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="P99" s="2"/>
       <c r="Q99" s="2"/>
@@ -7537,21 +7532,21 @@
       <c r="S99" s="2"/>
       <c r="T99" s="2"/>
       <c r="U99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="V99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="W99" s="2"/>
       <c r="X99" s="2"/>
       <c r="Y99" s="2"/>
       <c r="Z99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AA99" s="2"/>
       <c r="AB99" s="2"/>
       <c r="AC99" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="AD99" s="4"/>
       <c r="AE99" s="4"/>
@@ -7579,34 +7574,20 @@
       <c r="BA99" s="6"/>
     </row>
     <row r="100">
-      <c r="A100" s="11">
+      <c r="A100" s="15">
         <v>97.0</v>
       </c>
-      <c r="B100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="C100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="D100" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
       <c r="E100" s="2"/>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
-      <c r="I100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="J100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="K100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="L100" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
+      <c r="K100" s="12"/>
+      <c r="L100" s="12"/>
       <c r="M100" s="2"/>
       <c r="N100" s="2"/>
       <c r="O100" s="2"/>
@@ -7616,18 +7597,16 @@
       <c r="S100" s="2"/>
       <c r="T100" s="2"/>
       <c r="U100" s="2"/>
-      <c r="V100" s="2"/>
+      <c r="V100" s="12" t="s">
+        <v>153</v>
+      </c>
       <c r="W100" s="2"/>
       <c r="X100" s="2"/>
       <c r="Y100" s="2"/>
       <c r="Z100" s="2"/>
       <c r="AA100" s="2"/>
-      <c r="AB100" s="12" t="s">
-        <v>152</v>
-      </c>
-      <c r="AC100" s="12" t="s">
-        <v>152</v>
-      </c>
+      <c r="AB100" s="12"/>
+      <c r="AC100" s="12"/>
       <c r="AD100" s="4"/>
       <c r="AE100" s="4"/>
       <c r="AF100" s="4"/>
@@ -7654,172 +7633,232 @@
       <c r="BA100" s="6"/>
     </row>
     <row r="101">
-      <c r="A101" s="1"/>
-      <c r="B101" s="6"/>
-      <c r="C101" s="6"/>
-      <c r="D101" s="6"/>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="6"/>
-      <c r="H101" s="6"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="6"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="6"/>
-      <c r="M101" s="6"/>
-      <c r="N101" s="6"/>
-      <c r="O101" s="6"/>
-      <c r="P101" s="6"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="6"/>
-      <c r="S101" s="6"/>
-      <c r="T101" s="6"/>
-      <c r="U101" s="6"/>
-      <c r="V101" s="6"/>
-      <c r="W101" s="6"/>
-      <c r="X101" s="6"/>
-      <c r="Y101" s="6"/>
-      <c r="Z101" s="6"/>
-      <c r="AA101" s="6"/>
-      <c r="AB101" s="6"/>
-      <c r="AC101" s="6"/>
-      <c r="AD101" s="6"/>
-      <c r="AE101" s="6"/>
-      <c r="AF101" s="6"/>
-      <c r="AG101" s="6"/>
-      <c r="AH101" s="6"/>
-      <c r="AI101" s="6"/>
-      <c r="AJ101" s="6"/>
-      <c r="AK101" s="6"/>
-      <c r="AL101" s="6"/>
-      <c r="AM101" s="6"/>
-      <c r="AN101" s="6"/>
-      <c r="AO101" s="6"/>
-      <c r="AP101" s="6"/>
-      <c r="AQ101" s="6"/>
-      <c r="AR101" s="6"/>
-      <c r="AS101" s="6"/>
-      <c r="AT101" s="6"/>
-      <c r="AU101" s="6"/>
-      <c r="AV101" s="6"/>
-      <c r="AW101" s="6"/>
+      <c r="A101" s="17">
+        <v>98.0</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="C101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E101" s="2"/>
+      <c r="F101" s="2"/>
+      <c r="G101" s="2"/>
+      <c r="H101" s="2"/>
+      <c r="I101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="J101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="K101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="L101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="M101" s="2"/>
+      <c r="N101" s="2"/>
+      <c r="O101" s="2"/>
+      <c r="P101" s="2"/>
+      <c r="Q101" s="2"/>
+      <c r="R101" s="2"/>
+      <c r="S101" s="2"/>
+      <c r="T101" s="2"/>
+      <c r="U101" s="2"/>
+      <c r="V101" s="12"/>
+      <c r="W101" s="2"/>
+      <c r="X101" s="2"/>
+      <c r="Y101" s="2"/>
+      <c r="Z101" s="2"/>
+      <c r="AA101" s="2"/>
+      <c r="AB101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AC101" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="AD101" s="4"/>
+      <c r="AE101" s="4"/>
+      <c r="AF101" s="4"/>
+      <c r="AG101" s="4"/>
+      <c r="AH101" s="4"/>
+      <c r="AI101" s="4"/>
+      <c r="AJ101" s="4"/>
+      <c r="AK101" s="4"/>
+      <c r="AL101" s="4"/>
+      <c r="AM101" s="4"/>
+      <c r="AN101" s="4"/>
+      <c r="AO101" s="4"/>
+      <c r="AP101" s="4"/>
+      <c r="AQ101" s="4"/>
+      <c r="AR101" s="4"/>
+      <c r="AS101" s="4"/>
+      <c r="AT101" s="4"/>
+      <c r="AU101" s="4"/>
+      <c r="AV101" s="4"/>
+      <c r="AW101" s="4"/>
       <c r="AX101" s="6"/>
       <c r="AY101" s="6"/>
       <c r="AZ101" s="6"/>
       <c r="BA101" s="6"/>
     </row>
     <row r="102">
-      <c r="A102" s="1"/>
-      <c r="B102" s="6"/>
-      <c r="C102" s="6"/>
-      <c r="D102" s="6"/>
-      <c r="E102" s="6"/>
-      <c r="F102" s="6"/>
-      <c r="G102" s="6"/>
-      <c r="H102" s="6"/>
-      <c r="I102" s="6"/>
-      <c r="J102" s="6"/>
-      <c r="K102" s="6"/>
-      <c r="L102" s="6"/>
-      <c r="M102" s="6"/>
-      <c r="N102" s="6"/>
-      <c r="O102" s="6"/>
-      <c r="P102" s="6"/>
-      <c r="Q102" s="6"/>
-      <c r="R102" s="6"/>
-      <c r="S102" s="6"/>
-      <c r="T102" s="6"/>
-      <c r="U102" s="6"/>
-      <c r="V102" s="6"/>
-      <c r="W102" s="6"/>
-      <c r="X102" s="6"/>
-      <c r="Y102" s="6"/>
-      <c r="Z102" s="6"/>
-      <c r="AA102" s="6"/>
-      <c r="AB102" s="6"/>
-      <c r="AC102" s="6"/>
-      <c r="AD102" s="6"/>
-      <c r="AE102" s="6"/>
-      <c r="AF102" s="6"/>
-      <c r="AG102" s="6"/>
-      <c r="AH102" s="6"/>
-      <c r="AI102" s="6"/>
-      <c r="AJ102" s="6"/>
-      <c r="AK102" s="6"/>
-      <c r="AL102" s="6"/>
-      <c r="AM102" s="6"/>
-      <c r="AN102" s="6"/>
-      <c r="AO102" s="6"/>
-      <c r="AP102" s="6"/>
-      <c r="AQ102" s="6"/>
-      <c r="AR102" s="6"/>
-      <c r="AS102" s="6"/>
-      <c r="AT102" s="6"/>
-      <c r="AU102" s="6"/>
-      <c r="AV102" s="6"/>
-      <c r="AW102" s="6"/>
+      <c r="A102" s="17">
+        <v>99.0</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="C102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E102" s="2"/>
+      <c r="F102" s="2"/>
+      <c r="G102" s="2"/>
+      <c r="H102" s="2"/>
+      <c r="I102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="J102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="K102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="L102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="M102" s="2"/>
+      <c r="N102" s="2"/>
+      <c r="O102" s="2"/>
+      <c r="P102" s="2"/>
+      <c r="Q102" s="2"/>
+      <c r="R102" s="2"/>
+      <c r="S102" s="2"/>
+      <c r="T102" s="2"/>
+      <c r="U102" s="2"/>
+      <c r="V102" s="12"/>
+      <c r="W102" s="2"/>
+      <c r="X102" s="2"/>
+      <c r="Y102" s="2"/>
+      <c r="Z102" s="2"/>
+      <c r="AA102" s="2"/>
+      <c r="AB102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="AC102" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="AD102" s="4"/>
+      <c r="AE102" s="4"/>
+      <c r="AF102" s="4"/>
+      <c r="AG102" s="4"/>
+      <c r="AH102" s="4"/>
+      <c r="AI102" s="4"/>
+      <c r="AJ102" s="4"/>
+      <c r="AK102" s="4"/>
+      <c r="AL102" s="4"/>
+      <c r="AM102" s="4"/>
+      <c r="AN102" s="4"/>
+      <c r="AO102" s="4"/>
+      <c r="AP102" s="4"/>
+      <c r="AQ102" s="4"/>
+      <c r="AR102" s="4"/>
+      <c r="AS102" s="4"/>
+      <c r="AT102" s="4"/>
+      <c r="AU102" s="4"/>
+      <c r="AV102" s="4"/>
+      <c r="AW102" s="4"/>
       <c r="AX102" s="6"/>
       <c r="AY102" s="6"/>
       <c r="AZ102" s="6"/>
       <c r="BA102" s="6"/>
     </row>
     <row r="103">
-      <c r="A103" s="1"/>
-      <c r="B103" s="6"/>
-      <c r="C103" s="6"/>
-      <c r="D103" s="6"/>
-      <c r="E103" s="6"/>
-      <c r="F103" s="6"/>
-      <c r="G103" s="6"/>
-      <c r="H103" s="6"/>
-      <c r="I103" s="6"/>
-      <c r="J103" s="6"/>
-      <c r="K103" s="6"/>
-      <c r="L103" s="6"/>
-      <c r="M103" s="6"/>
-      <c r="N103" s="6"/>
-      <c r="O103" s="6"/>
-      <c r="P103" s="6"/>
-      <c r="Q103" s="6"/>
-      <c r="R103" s="6"/>
-      <c r="S103" s="6"/>
-      <c r="T103" s="6"/>
-      <c r="U103" s="6"/>
-      <c r="V103" s="6"/>
-      <c r="W103" s="6"/>
-      <c r="X103" s="6"/>
-      <c r="Y103" s="6"/>
-      <c r="Z103" s="6"/>
-      <c r="AA103" s="6"/>
-      <c r="AB103" s="6"/>
-      <c r="AC103" s="6"/>
-      <c r="AD103" s="6"/>
-      <c r="AE103" s="6"/>
-      <c r="AF103" s="6"/>
-      <c r="AG103" s="6"/>
-      <c r="AH103" s="6"/>
-      <c r="AI103" s="6"/>
-      <c r="AJ103" s="6"/>
-      <c r="AK103" s="6"/>
-      <c r="AL103" s="6"/>
-      <c r="AM103" s="6"/>
-      <c r="AN103" s="6"/>
-      <c r="AO103" s="6"/>
-      <c r="AP103" s="6"/>
-      <c r="AQ103" s="6"/>
-      <c r="AR103" s="6"/>
-      <c r="AS103" s="6"/>
-      <c r="AT103" s="6"/>
-      <c r="AU103" s="6"/>
-      <c r="AV103" s="6"/>
-      <c r="AW103" s="6"/>
+      <c r="A103" s="17">
+        <v>100.0</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="C103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="E103" s="2"/>
+      <c r="F103" s="2"/>
+      <c r="G103" s="2"/>
+      <c r="H103" s="2"/>
+      <c r="I103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="J103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="K103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="L103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="M103" s="2"/>
+      <c r="N103" s="2"/>
+      <c r="O103" s="2"/>
+      <c r="P103" s="2"/>
+      <c r="Q103" s="2"/>
+      <c r="R103" s="2"/>
+      <c r="S103" s="2"/>
+      <c r="T103" s="2"/>
+      <c r="U103" s="2"/>
+      <c r="V103" s="12"/>
+      <c r="W103" s="2"/>
+      <c r="X103" s="2"/>
+      <c r="Y103" s="2"/>
+      <c r="Z103" s="2"/>
+      <c r="AA103" s="2"/>
+      <c r="AB103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC103" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD103" s="4"/>
+      <c r="AE103" s="4"/>
+      <c r="AF103" s="4"/>
+      <c r="AG103" s="4"/>
+      <c r="AH103" s="4"/>
+      <c r="AI103" s="4"/>
+      <c r="AJ103" s="4"/>
+      <c r="AK103" s="4"/>
+      <c r="AL103" s="4"/>
+      <c r="AM103" s="4"/>
+      <c r="AN103" s="4"/>
+      <c r="AO103" s="4"/>
+      <c r="AP103" s="4"/>
+      <c r="AQ103" s="4"/>
+      <c r="AR103" s="4"/>
+      <c r="AS103" s="4"/>
+      <c r="AT103" s="4"/>
+      <c r="AU103" s="4"/>
+      <c r="AV103" s="4"/>
+      <c r="AW103" s="4"/>
       <c r="AX103" s="6"/>
       <c r="AY103" s="6"/>
       <c r="AZ103" s="6"/>
       <c r="BA103" s="6"/>
     </row>
     <row r="104">
-      <c r="A104" s="1"/>
+      <c r="A104" s="11"/>
       <c r="B104" s="6"/>
       <c r="C104" s="6"/>
       <c r="D104" s="6"/>

</xml_diff>